<commit_message>
Integration in excel file wip
</commit_message>
<xml_diff>
--- a/Boti_Consolidado_octubre_2025.xlsx
+++ b/Boti_Consolidado_octubre_2025.xlsx
@@ -73,7 +73,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -85,6 +85,12 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -687,10 +693,8 @@
           <t>Mide el porcentaje de usuarios que lograron su objetivo</t>
         </is>
       </c>
-      <c r="D14" s="4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D14" s="5" t="n">
+        <v>0.6127811275912152</v>
       </c>
     </row>
     <row r="15" ht="25" customHeight="1">
@@ -704,10 +708,8 @@
           <t>Mide la facilidad con la que los usuarios pueden interactuar</t>
         </is>
       </c>
-      <c r="D15" s="4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D15" s="6" t="n">
+        <v>2.342400814482517</v>
       </c>
     </row>
     <row r="16" ht="25" customHeight="1">
@@ -721,10 +723,8 @@
           <t>Mide la satisfacción usando una escala de 1 a 5</t>
         </is>
       </c>
-      <c r="D16" s="4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D16" s="5" t="n">
+        <v>0.6788680632120544</v>
       </c>
     </row>
     <row r="17" ht="25" customHeight="1">
@@ -738,7 +738,7 @@
           <t>Disponibilidad del servidor (% tiempo activo)</t>
         </is>
       </c>
-      <c r="D17" s="4" t="inlineStr">
+      <c r="D17" s="5" t="inlineStr">
         <is>
           <t>100.0%</t>
         </is>

</xml_diff>